<commit_message>
Updated filtering criteria to filter on the basis of a single keyword only
</commit_message>
<xml_diff>
--- a/Employment.xlsx
+++ b/Employment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
   <x:si>
     <x:t>Title</x:t>
   </x:si>
@@ -49,236 +49,132 @@
     <x:t>Requirements</x:t>
   </x:si>
   <x:si>
-    <x:t>Materials Scientist BD
-              Franklin Lakes, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">devicesQualificationsRequired qualifications:PhD: 0-3 years of post-graduate industrial QualificationsMedical device industry </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">products.ResponsibilitiesThe candidate is expected to possess a deep understanding of the linkage between molecular architecture and structure, resin formulation of polymer blends, resin processing, and properties for a broad range of polymer materials, with preference for those with skill sets in either sustainable materials technology or formulation design of thermoplastic elastomers (TPE). The candidate should be able to:Work as an individual contributor in a multidisciplinary team.Define material properties and </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experience or knowledge in the transfer of technology into design and manufacturing of experience or an equivalent combination of education and experienceDegree: Chemistry, polymer science, chemical engineering, materials science, or other related degreesSuccessful track record of on time delivery to project deliverablesDesired experience desiredExperience in environmentally sustainable materials or polymeric based sensor materialsDemonstrated understanding of material structure-property relationshipApplication of statistical and analytical methods of analysisAn understanding of design control processesExperience with scale-up and transfer of material technologies to manufacturingTest protocol generation, execution, and reportingExcellent verbal and written communication skillsBasic knowledge of project management for new product developmentAbility to work within multifunctional teams and work cross-functionally.A basic understanding of regulatory and quality processesFor certain roles at BD, employment is contingent upon the Company’s receipt of sufficient proof that you are fully vaccinated against COVID-19. In some locations, testing for COVID-19 may be available and/or required. Consistent with BD’s Workplace Accommodations Policy, requests for accommodation will be considered pursuant to applicable law.Why join us?A career at BD means being part of a team that values your opinions and contributions and that empowers you to bring your authentic self to work. Here our associates can fulfill their life’s purpose through the work that they do every day.You will learn and work alongside inspirational leaders and colleagues who are equally passionate and committed to fostering an inclusive, growth-centered, and rewarding culture. Our Total Rewards program — which includes competitive pay, </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">benefits, continuous learning, recognition, career growth, and life balance components — is designed to support the varying needs of our diverse and global associates.To learn more about BD visit https://jobs.bd.com/Becton, Dickinson and Company is an Equal Opportunity/Affirmative Action Employer. We do not unlawfully discriminate on the basis of race, color, religion, age, sex, creed, national origin, ancestry, citizenship status, marital or domestic or civil union status, familial status, affectional or sexual orientation, gender identity or expression, genetics, disability, military eligibility or veteran status, or any other protected status.PDNPrimary Work LocationUSA NJ - Franklin LakesAdditional LocationsWork Shift Show more Show less </x:t>
+    <x:t>Grand Junction Elementary School Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">experience. Show more Show less </x:t>
   </x:si>
   <x:si>
     <x:t>Full-time</x:t>
   </x:si>
   <x:si>
+    <x:t>Entry level</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction Elementary School Reading Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction Elementary School Science Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction Elementary School Writing Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction Elementary School Math Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction Middle School Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction High School Level American History Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Not Applicable</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">requirements to meet product requirements.Excellent communication skills both written and oral to effectively communicate with cross-functional team members.Keep abreast of potential new technologies.Leverage existing technologies to advance our core businesses while supporting the development of new products and platforms. Collaborate in the creation, evaluation, and assessment of competitive products, processes, technology, and trends. Ensure compliance with BD quality policies, procedures, and practices through appropriate communication, training, and education of sound quality assurance principles. Design, develop, and improve materials related to BD productsImplement experimental designs, write protocols and reports, perform data analysis, present out on findingsProvide direction to junior engineers and technicians where appropriate.Assist in the transfer of new technologies from R&amp;D to manufacturingActively seek training to improve skills and teach/promote/reward new learning within the organizationStrong fit within BD’s core valuesHighly Desirable Skills IncludeAdvancement of sustainable materials technology through chemistry development, polymer synthesis, material science, and fostering relationships and collaborations in sustainable material technology space.Formulation, design, and compounding of thermoplastic elastomer technologyApplications of polymer or material science in the design and manufacture of medical </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chemist (Flavor &amp; Fragrance) Coda Search│Staffing
-              Totowa, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experienced chemist with a strong background in organic and process chemistry to develop new products and processes for flavor and fragrance ingredients for the food and cosmetics industry. Successful applicant will have excellent theoretical and practical knowledge as well as experience in organic synthesis including synthetic methodology, catalysis, upstream and downstream processing. The position also requires conceptual design and experimental validation of designed processes. Other Experience in distillation, re-crystallization, sublimation, deposition and extractions, synthesis- Two years of industrial experience or related- Knowledge of various lab equipment- Ability to design, execute and troubleshoot experiments and processes- Capacity to work independently- Possess strong written and oral communication skills- Ability to work effectively in a team environment and individually- Physical fitness is required Show more Show less </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mid-Senior level</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">requirements:- Bachelor or Master Degree in organic chemistry or related field- </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Materials Scientist 1 MillenniumSoft Inc
-              Franklin Lakes, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Qualifications B.S. + degree in Materials Science, Chemistry, or related disciplines Good understanding of material structure-property relationships Hands-on Qualifications M.S. or Ph.D. degree in Material Science, chemistry, or related discipline </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experience with analytical or material characterization instrumentation such as INSTRON, DSC/TGA, DMA and FTIR, UV-VIS Hands-on experience with wet laboratory equipment and skills. Strong inter-personal and communication skillsPreferred Experience and knowledge in blood biology and clinical assays Proficient with Minitab Experience in design of experiments Excellent written and verbal communication skills as well as ability to communicate effectively with scientists and engineers from a wide range of technical backgrounds. Show more Show less </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Associate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Materials Scientist MillenniumSoft Inc
-              Franklin Lakes, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">responsibilities: Work cross-functionally to improve product from quality and compliance perspective Conduct material characterizations to support material supply risk mitigation projects Perform mechanical test of final assembled blood collection tube products and report results to principle investigator and/or project team Develop analytical testing methods Develop and execute test protocols and document results in a timely fashion Coordinate bio-compatibility testing Review documentation for accuracy Maintenance of equipment and laboratory facilities Show more Show less </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Experience PreferredMain job </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Raw Material Chemist Kelly
-              Northvale, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">cGMP.Qualifications Minimum of a bachelor’s degree in a science-related field, preferably Chemistry. 2-3 years of </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">responsibility is to perform routine release testing of raw materials (Active ingredient, excipients, colors,) and packaging materials in accordance with established procedures (in-house, Pharmacopeia, vendor procedures) Perform routine tests as assays, related compounds, chromatographic purity, residual solvents, particle size distribution, Infrared spectroscopy using different techniques and instrumentation like FTIR, UV, HPLC, UPLC, GC, etc. Perform routine wet chemistry analysis as titrations, water content, specific rotation, melting point, identification tests, viscosity, density, LOD, LOI, ROI etc. as per respective monographs and established procedures in a regulated laboratory environment. Evaluates test results and determines acceptability of the data based on acceptance criteria. Reviewing and releasing of the raw data, documentation and results for certificate of analysis. Writing technical documents like specifications, analytical methods, method verification protocols and reports, method transfer documents, investigation reports etc. Maintain accurate lab notebooks and complete all related analytical reports, write summaries, and maintain proper GMP documentation in compliance with SOPs. Design and develop test methods, perform experimental tests and evaluate performances of test methods. Establish test specifications, communicates with internal and external customers. Follow all SOPs and Safety Guidelines to ensure compliance with a cGMP environment and Safety Practices. Maintain the laboratories with good housekeeping practices and in compliant with </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experience in either raw material or finished product testing Proficiency in use of software including Microsoft Word and Microsoft Excel. Good communication and writing skillsYou should know:* Your safety matters! Vaccination against COVID-19 may be a </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">[benefits](https://www.mykelly.us/us-mykelly/perks/)?). Connecting great people with great companies is what we do best, and our employment opportunities span a wide variety of workstyles, skill levels, and industries around the world.Kelly is an equal opportunity employer committed to employing a diverse workforce, including, but not limited to, minorities, females, individuals with disabilities, protected veterans, sexual orientation, gender identity. [Equal Employment Opportunity is The Law.](https://www.dol.gov/ofccp/regs/compliance/posters/ofccpost.htm) Show more Show less Seniority level Associate Employment type Full-time Job function Research, Analyst, and Information Technology Industries Staffing and Recruiting </x:t>
-  </x:si>
-  <x:si>
-    <x:t>$49,000.00/yr - $80,000.00/yr</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">requirement for this job in compliance with current client and governmental policies. A Kelly recruiter will confirm and share more details with you during the interview process.Why Kelly®?Kelly® Science &amp; Clinical is your connection to premier scientific and clinical companies looking to hire talented people just like you. Every day, we match science professionals with dream jobs that fit their skills and interests—it’s the way we think job searching should be. Nearly 100 percent of our science recruiters have a professional background/education in science, so we know a thing or two about the science market and how to get you noticed.About Kelly®At Kelly, we’re always thinking about what’s next and advising job seekers on new ways of working to reach their full potential. In fact, we’re a leading advocate for temporary/nontraditional workstyles, because we believe they allow flexibility and tremendous growth opportunities that enable a better way to work and live (plus, did we mention we provide a ton of </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sr. Staff Scientist – Materials, Sustainability BD
-              Franklin Lakes, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">QualificationsMinimum of a master’s degree in chemistry, chemical engineering, or associated medical technology field.Ph.D. preferred 10+ years work </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">responsibilities when required.Job DescriptionBe part of something bigger!BD is one of the largest global medical technology companies in the world and is advancing the world of health by improving medical discovery, diagnostics and the delivery of care. We have over 65,000 employees and a presence in virtually every country around the world to address some of the most challenging global health issues.Scope And ResponsibilitiesThis is a key role in the Sustainable Medical Technology Institute (SMTI) and this individual will serve as the subject matter expert on topics related to materials of construction of BD products. It entails materials related activities in all three focus areas within the SMTI, namely Materials of Concern, Sterilization, and Design for Sustainability. The individual will be responsible for leading and driving new material technology programs, to enable product differentiation to meet current and future unmet needs, and engage with stakeholder across Business Units (BU).The candidate should have previous responsibilities with high complexity or high innovation to BD technology, products, systems, organization, or services. Regular interaction and collaboration with R&amp;D and project team members within each Business Unit is critical for the successful execution of responsibilities since this candidate will help with material selection for products developed and commercialized by these teams. The individual will also work closely with the Integrated Supply Chain (ISC) team, more specifically procurement, to establish and maintain an overview of BD-wide materials as they pertain to the SMTI mandate. This can include regular interaction with vendors. Interactions frequently involve detailed knowledge of industry practices across medical technology, specialty materials, transport, pharmaceutical, and hospital network categories which BD must use to satisfy sustainability responsibility of this role requires the individual to stay abreast with new technologies in the materials field, to leverage external resources to augment BD’s internal materials development. This is enabled via a strong engagement with industry leaders and academic programs. Previous demonstrated </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experience with materials, and material selection for medical devices. He/she should have an established track record of solving complex issues where analysis of situations or data requires an in-depth knowledge of materials science, and material property-product performance correlation. Additionally, he/she must possess a solid understanding of structure property relationships and knowledge of polymers / resin manufacture and processing. The candidate will utilize this expertise to develop and deploy methods, techniques, and evaluation criteria for achieving BD’s sustainability goals. He/she will build on this by identification of appropriate material testing, getting it executed where appropriate and interfacing with product development groups for selection of materials of construction.This position will be accountable for experience with identification of external material technologies followed by implementation into product development is highly desirable.Impact Of This RoleDecisions made by the person in this role will have serious impact on the overall success or failure of BD’s sustainability goals and business goals. Erroneous decision or recommendations may cause critical delays or modification to company projects or operations causing substantial expenditure of time, human resources, and funds. Development of robust recommendations based on solid scientific reasoning, including experimentation where required, and ability to communicate this with critical stakeholders within each Business Unit will be critical to success in this role. The candidate should have a demonstrated ability to work effectively in a matrixed environment, and should be willing to provide examples of the same.Education &amp; experience focused on use of polymers in medical devices required, with focus on polymeric materials selection leading to implementation into product development activities is highly desired. The Candidate Will PossessSolid understanding of polymer architecture, resin formulation, processing and chemical &amp; physical properties Experience translating customer needs and product performance </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">benefits, continuous learning, recognition, career growth, and life balance components — is designed to support the varying needs of our diverse and global associates.To learn more about BD visit https://jobs.bd.com/Becton, Dickinson and Company is an Equal Opportunity/Affirmative Action Employer. We do not unlawfully discriminate on the basis of race, color, religion, age, sex, creed, national origin, ancestry, citizenship status, marital or domestic or civil union status, familial status, affectional or sexual orientation, gender identity or expression, genetics, disability, military eligibility or veteran status, or any other protected status.PDNPrimary Work LocationUSA NC - Research Triangle ParkAdditional LocationsUSA NJ - Franklin LakesWork Shift Show more Show less </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">requirements. May negotiate with suppliers, providers, vendors to influence purchasing and operational strategies for BD. Influences and advises senior level leaders regarding matters of significance to the organization.Another important requirements into material property requirementsTrack record of material selection to accommodate design and manufacturing requirementsInnovative mindset with follow through on the translation the innovation into products and manufacturingGeneral project management skills with ability to manage efforts across multiple projectsAbility to lead cross-functional teams and mentor associatesWillingness to travel globally up to 20% For certain roles at BD, employment is contingent upon the Company’s receipt of sufficient proof that you are fully vaccinated against COVID-19. In some locations, testing for COVID-19 may be available and/or required. Consistent with BD’s Workplace Accommodations Policy, requests for accommodation will be considered pursuant to applicable law.Why join us?A career at BD means being part of a team that values your opinions and contributions and that empowers you to bring your authentic self to work. Here our associates can fulfill their life’s purpose through the work that they do every day.You will learn and work alongside inspirational leaders and colleagues who are equally passionate and committed to fostering an inclusive, growth-centered, and rewarding culture. Our Total Rewards program — which includes competitive pay, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Process Chemistry Scientist Kallyope
-              New York, NY</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">environmentQualifications And Education </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ResponsibilitiesSupport medicinal chemistry by overcoming synthetic roadblocks to chemical intermediates and active pharmaceutical ingredients (API) and streamlining SARDesign and perform experiments to enable new route design and development/implementation of phase appropriate and robust synthetic processes to successfully facilitate the delivery of preclinical and clinical API batches at CDMOsManage vendor / CDMO teams conducting scale-up activities to deliver API required for IND-enabling studiesSummarize and present experimental results to the project team to facilitate strategic planning, risk-assessment, and decision-making in a collaborative team </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experience in scale-up of API, from discovery to the clinic, and managing external partners. While this is a lab-focused position, the right candidate can work remotely, depending on experience. Successful candidates must be able to work effectively both in a collaborative setting and independently, while possessing outstanding written, visual and oral communications skills.Key experience, with an emphasis on developing chemical processesFamiliarization with modern process chemistry techniques: crystallization development, route/step optimization, HPLC analysis and assay, process safety and impurity controlExperience managing external partnersExceptional problem-solving skills and ability to quickly adapt and shift focus as neededExcellent interpersonal, communication, and collaboration skillsAbility to multi-task in a fast-paced dynamic environment while demonstrating a calm and positive attitude and a superior work ethicAbout KallyopeKallyope is a new biotechnology company headquartered in New York City. Founded by Richard Axel, Tom Maniatis, and Charles Zuker from Columbia University, Kallyope is focused on the identification of new therapeutic and nutritional opportunities involving the gut and gut-brain axis. The Company leverages the founders' formidable expertise in molecular biology, neuroscience, and behavior to identify new approaches to human health.Kallyope is seeking creative, highly motivated individuals who are interested in working in a biotech environment that is scientifically stimulating, highly collaborative, and laser focused on translational biology. The Company is creating an industry-leading platform employing cutting edge technologies including sequencing, genetics, circuit mapping, neural imaging and bioinformatics. By integrating and applying complementary tools and approaches to the understanding of gut and gut-brain biology, Kallyope aims to develop transformational therapeutics and consumer products to improve human health and nutrition.The Company is headquartered in the Alexandria Center® for Life Sciences, a state-of-the-art, collaborative life science campus in the heart of Manhattan, with close proximity to New York City's world-leading clinical and research institutions. Kallyope has raised $252M in funding from several top-tier investors. The Company has assembled a leadership team and advisory group with a proven track record of success and strong expertise in drug discovery and translation. The founding scientific team is composed of highly creative and talented individuals with outstanding expertise in the Company's core platform technologies. For more information, see www.kallyope.com. Show more Show less Seniority level Associate Employment type Full-time Job function Research, Analyst, and Information Technology Industries Biotechnology Research </x:t>
-  </x:si>
-  <x:si>
-    <x:t>$84,000.00/yr - $139,000.00/yr</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">RequirementsYou must have:M.Sc. or higher degree in organic chemistry with 5+ years of drug discovery/development </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chemist- Cementitious Sika
-              Lyndhurst, NJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Responsibilities- Responsible for managing assigned projects (from Idea Proposal to Product Release) Independently develop new products according to customer specifications. Develop DOE and Design FEMA for product development. Participate in 3-year or long-term product/technology planning Evaluate new testing instrument and make recommendations for capital expenditures. Define new product QA </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Chemists.Qualifications/Experience/Education- BS or MS degree in Chemistry, Polymer Science or Chemical Engineering or similar. 2+ years hand-on industrial experience in cement chemistry or cementitious based formulations. Strong presentation skills. Excellent technical and business writing skills. Excellent skills in DOE, Design FEMA, other quality programs. Good computer skills in Microsoft Word, Excel, Power Point and Project Management.Building Trust Every DayTrust is the foundation of everything we do at Sika- we trust in the skills, expertise and capabilities of all our employees.Built on a foundation of pioneering and entrepreneurial spirit, Sika empowers its people to propose and develop new ideas.Job CategoryChemistry / Research &amp; Development / LaboratoryJob ID10919BR Show more Show less </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">requirements to ensure product quality and performance. Responsible for transferring new products/technologies to the Processing group. Perform initial material testing and gain material approvals from customers. Provide technical support to manufacturing plant to assure product quality. Support internal procedures, PCP and ISO processes. Keep accurate records and maintain good laboratory notebook practice. Publish Research Proposals, Field Trial Proposals and Product Releases as required. Publish progress reports, trip reports and monthlies on approved projects. Visit customer sites and provide technical solutions to customers. Initiate and attend technical presentation from raw material suppliers. Maintain a safe, tidy and harassment free work environment Maintain assigned equipment in a good operating condition. Provide training to new employees, technicians or Junior </x:t>
-  </x:si>
-  <x:si>
-    <x:t>General Cleaner IH Services, Inc.
-              Gene Autry, OK</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">neededQualificationsMust pass drug screen and background check and have reliable transportationA strong work ethic The ability to work alone or within a team is a must.JOB CODE: 1126 Show more Show less </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Part-time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Entry level</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Environmental Svc Tech I Mercy</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">schedules; maintains a high level of cleanliness at all times according to established procedures. Creates a clean and safe environment for Mercy Memorial Center customers through the proper disposal of hospital waste. Will perform all work with accord to the mission, vision, and values of Mercy. </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Qualifications: </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Experience: Housekeeping skills preferred, but not required. Must have good communication skills both oral and written Other: Must have good communication skills both oral and written. We Offer Great experience through advanced technology and innovative procedures. We're expanding to help our communities grow. Join us and be a part of it all. What Makes You a Good Match for Mercy? Compassion and professionalism go hand-in-hand with us. Having a positive outlook and a strong sense of advocacy is in perfect step with our mission and vision. We're also collaborative and unafraid to do a little extra to deliver excellent care - that's just part of our commitment. If that sounds like a good fit for you, we encourage you to apply. EVS, housekeeping, maid, cleaning Mercy has determined this is a safety-sensitive position. The ability to work in a constant state of alertness and in a safe manner is an essential function of this job. Hiring InsightsJob activityPosted 3 days ago </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Health insuranceDental insuranceTuition reimbursementPaid time offVision insurance TypeFull-timeBenefitsPulled from the full job descriptionHealth insuranceDental insuranceTuition reimbursementPaid time offVision insuranceFull Job Description We're a Little Different Our mission is clear. We bring to life a healing ministry through our compassionate care and exceptional service. At Mercy, we believe in careers that match the unique gifts of unique individuals - careers that not only make the most of your skills and talents, but also your heart. Join us and discover why Modern Healthcare Magazine named us in its "Top 100 Places to Work." Overview: Under the direct supervision of the Supervisor, does general cleaning and housekeeping duties in assigned area and in accordance with Benefits: Day-one comprehensive health, vision and dental coverage, PTO, tuition reimbursement and employer-matched retirement funds are just a few of the great benefits offered to eligible co-workers, including those working 48 hours or more per pay period! We're bringing to life a healing ministry through compassionate care. At Mercy, our supportive community will be behind you every step of your day, especially the tough ones. You will have opportunities to pioneer new models of care and transform the health care </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Environ Svc Floor Tech Mercy</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">schedules; maintain a high level of cleanliness at all times according to established procedures. </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Qualifications: Education: High School Education or equivalent preferred, but not required. Other Skills and Knowledge: Floor care </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experience on different types of floor. Good communication skills. Good Organizational Skills. We Offer Great experience through advanced technology and innovative procedures. We're expanding to help our communities grow. Join us and be a part of it all. What Makes You a Good Match for Mercy? Compassion and professionalism go hand-in-hand with us. Having a positive outlook and a strong sense of advocacy is in perfect step with our mission and vision. We're also collaborative and unafraid to do a little extra to deliver excellent care - that's just part of our commitment. If that sounds like a good fit for you, we encourage you to apply. Mercy has determined this is a safety-sensitive position. The ability to work in a constant state of alertness and in a safe manner is an essential function of this job. Hiring InsightsJob activityPosted 4 days ago </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Health insuranceDental insuranceTuition reimbursementPaid time offVision insurance TypeFull-timeBenefitsPulled from the full job descriptionHealth insuranceDental insuranceTuition reimbursementPaid time offVision insuranceFull Job Description We're a Little Different Our mission is clear. We bring to life a healing ministry through our compassionate care and exceptional service. At Mercy, we believe in careers that match the unique gifts of unique individuals - careers that not only make the most of your skills and talents, but also your heart. Join us and discover why Modern Healthcare Magazine named us in its "Top 100 Places to Work." Overview: Under the direct supervision of the Supervisor, does general floor cleaning and maintance duties in assigned area and in accordance with Benefits: Day-one comprehensive health, vision and dental coverage, PTO, tuition reimbursement and employer-matched retirement funds are just a few of the great benefits offered to eligible co-workers, including those working 48 hours or more per pay period! We're bringing to life a healing ministry through compassionate care. At Mercy, our supportive community will be behind you every step of your day, especially the tough ones. You will have opportunities to pioneer new models of care and transform the health care </x:t>
-  </x:si>
-  <x:si>
-    <x:t>General Cleaner IH Services</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Health insuranceDental insurancePaid time offEmployee assistance programVision insurance </x:t>
-  </x:si>
-  <x:si>
-    <x:t>$12 an hour</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Retail Custodian Love's Travel Stops &amp; Country Stores</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">scheduleLife insuranceFull Job Description Req ID: 320605 Store Maintenance Technician Maintenance Tech′s help run our business by keeping a safe, clean and well-maintained stop. You′ll also help your manager keep things flowing and get our customers back on the road quickly. We take a lot of pride in making customers want to come back and your work makes a big difference. We have a lot to offer Flexible Schedule Competitive pay (paid weekly) Holiday pay Medical/Dental/Vision and Life Insurance Plans Career development programs 401(k) with matching contributions Hourly Bonus Program (Golden Hearts) Many types of training opportunities Do′ers Welcome We′re do′ers. We get the job done. We solve problems when they come up and we work like a team. Love′s will always have your back too. We′ve had more job and career success stories than we can list. Promotions, rewards, raises, great schedule that could include some nights, days, weekends and even some holidays? Diversity Statement. From the founding of Love’s, our leaders have been passionate about providing excellent customer </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">experiences and helping our Team Members grow. We do both within a culture of respect and inclusion. In order to sustain this culture, we will welcome individuals who are diverse in experiences, age, race, gender, sexual orientation, religion and physical or mental ability. Also, we are committed to sustaining a professional working environment where ALL people feel respected. By doing these things we will cultivate diversity of thought and a spirit of innovation. Join us on the Road to Success. We want everyone who joins the Love′s family to succeed and we mean that! Our Road to Success Program was created for you. We provide leadership and management skills training and full apprenticeships for those just starting out. Once you′re a manager, the training goes even further with a two day workshop at Love′s University. There you′ll experience dynamic days with other managers and leaders, including our CEO Tom Love and senior executives. Our Road to Success program is such a valuable experience for career growth and for you personally, we wish the whole country could participate. Job Function(s): Retail Love’s Travel Stops &amp; Country Stores is the industry-leading travel stop network in the United States. For more than 55 years, we’ve provided customers with highway hospitality and “Clean Places, Friendly Faces.” We’re passionate about serving drivers with clean, modern facilities stocked with fuel, food and supplies. We offer meals from popular restaurant chains, trucking supplies, showers and everything needed to get back on the road quickly. The Love’s Family of Companies includes: Gemini Motor Transport, one of the industry’s safest trucking fleets Speedco, the light mechanical and trucking service specialists Musket, a rapidly growing, Houston-based commodities supplier and trader Trillium, a Houston-based alternative fuels expert
-Hiring InsightsJob activityPosted 30+ days ago </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Health insuranceDental insurance401(k)Paid time offVision insurance401(k) matchingFlexible scheduleLife insurance weeklyBenefitsPulled from the full job descriptionHealth insuranceDental insurance401(k)Paid time offVision insurance401(k) matchingFlexible benefits and a ton of respect all can come true at Love′s. It starts with “I can do it”. Let′s get you started. If you′re good with our physical </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">requirements, we′d really like to hear from you. You might have to lift and move equipment around that could weigh up to 50lbs. Is that a problem? We′re on our feet a lot and an 8 hour shift could be all standing. Would you be ok standing for long periods? Can you work a flexible </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nurse Technician-NT - Ardmore 2nd Floor - PRN/Days Mercy</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Qualifications: Education: High school diploma, G.E.D. and enrolled in a board-certified nursing program. Prior to employment, the nurse tech shall provide student transcripts indicating they have completed Fundamentals of Nursing from an accredited school of nursing and provide competency skills list from their learning institution. The nurse tech must remain in good standing with their school of nursing while in this role. This program is for nursing students only, if a student leaves a program for any reason, they can no longer be a nurse tech. Certifications: BLS Required within one month of hire Other: Minimum Physical </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Experience: EMT, Paramedic or Previous Patient Care Experience Preferred Certifications: Certified Nursing Assistant (CNA), Certified Patient Care Tech (CPCT), Emergency Medical Technician (EMT), Advanced Unlicensed Assistant (AUA) in the State of Oklahoma. We Offer Great experience through advanced technology and innovative procedures. We're expanding to help our communities grow. Join us and be a part of it all. What Makes You a Good Match for Mercy? Compassion and professionalism go hand-in-hand with us. Having a positive outlook and a strong sense of advocacy is in perfect step with our mission and vision. We're also collaborative and unafraid to do a little extra to deliver excellent care - that's just part of our commitment. If that sounds like a good fit for you, we encourage you to apply. Mercy has determined this is a safety-sensitive position. The ability to work in a constant state of alertness and in a safe manner is an essential function of this job. Hiring InsightsJob activityPosted 2 days ago </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Health insuranceDental insuranceTuition reimbursementPaid time offVision insurance TypePRNBenefitsPulled from the full job descriptionHealth insuranceDental insuranceTuition reimbursementPaid time offVision insuranceFull Job Description We're a Little Different Our mission is clear. We bring to life a healing ministry through our compassionate care and exceptional service. At Mercy, we believe in careers that match the unique gifts of unique individuals - careers that not only make the most of your skills and talents, but also your heart. Join us and discover why Modern Healthcare Magazine named us in its "Top 100 Places to Work." Overview: Under the direction of the RN or LPN, assists in the individualized care of the patient to achieve the patient's highest level of wellness. Works cooperatively with others as part of a team; recognizes the importance of group goals. Performs designated clinical procedures and nonclinical support tasks essential to providing care to the patient. Benefits: Day-one comprehensive health, vision and dental coverage, PTO, tuition reimbursement and employer-matched retirement funds are just a few of the great benefits offered to eligible co-workers, including those working 48 hours or more per pay period! We're bringing to life a healing ministry through compassionate care. At Mercy, our supportive community will be behind you every step of your day, especially the tough ones. You will have opportunities to pioneer new models of care and transform the health care </x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRN</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Requirements Position requires individuals to push, pull, and/or lift 50 pounds on a regular basis Position requires prolonged standing and walking each shift Position requires the ability to grip, reach, bend, kneel, twist, and squat to perform duties Preferred </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Housekeeper, Maid </x:t>
-  </x:si>
-  <x:si>
-    <x:t>$8.00 - $8.50 an hour</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Industrial Cleaning Technician Johnston Cleaning</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$15 an hour</x:t>
+    <x:t>Grand Junction Middle School Reading Comprehension Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction Middle School Reading Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grand Junction High School Biology Certified Teacher Varsity Tutors, a Nerdy Company
+              Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BOOKCLIFF CHRISTIAN SCHOOL 4th Grade Classroom Teacher Grand Junction, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">scheduled devotional, in-service, retreat, committee, faculty, and Parent Teacher Fellowship meetings.23. Know the procedures for dealing with issues of an emergency nature.24. Inform the administration, in a timely manner if unable to fulfill any duty assigned.25. Prepare adequate information materials for a substitute teacher and maintain an emergency substitute folder.This teacher teaches elementary students academic, social, and motor skills using Christian based material and prepares course objectives and outlines for course of study following the curriculum guidelines (deviations from assigned curriculum must have administrative approval.) Lectures, demonstrations, and use of audiovisual teaching aids to present subject matter are employed. The teacher prepares, administers, and corrects tests, daily work, oral presentations, and extra credit assignments and records results, teaches Christian values and Biblical teachings, maintains order in the classroom and on the playground, counsels pupils when adjustments on behavior and academic problems arise using God's word, discusses pupils' academic and behavioral attitudes and achievement with parents, keeps attendance and grade records, and coordinates class field trips.Job Type: offSchedule:Monday to FridayEducation:Bachelor's </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">(Preferred)Experience:Teaching: 1 year (Preferred)License/Certification:Teaching Certification (Preferred)Work Location: One location </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Full-timeBenefits:Health insurancePaid time </x:t>
+  </x:si>
+  <x:si>
+    <x:t>$29,750 /yr (est.)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garfield School District Re-2 1st Grade Teacher Rifle, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">experience, and continuing education credits. For out of District experience, the District can honor up to 10 years of out of District experience towards salary credit. Credits for salary advancement can be obtained through professional development, or completing graduate level courses.
+Garfield Re-2 School District offers </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">benefits including medical, dental, and vision coverage, prescription drug coverage, medical and dependent care flexible spending accounts, metlife products, employee assistance programs, surgery plus opportunities, paid time off, sick leave, vacation leave, holiday pay, PERA retirement plan, identity theft protection, local discounts, Verizon Wireless discount, and more.
+EEO Statement:
+Garfield School District RE-2 is an Equal Opportunity Employer and Educator who fully and actively supports equal access for all people in admission or access to, or treatment or employment in its programs and activities, regardless of race, color, religion, gender, age, national origin, veteran status, disability, genetic information or testing, sexual orientation, and gender identity or expression. We prohibit retaliation against individuals who bring forth any complaint, orally or in writing, to the employer of the government, or against any individuals who assist or participate in the investigation of any complaint, or otherwise oppose discrimination. Any person having inquiries concerning the School's compliance with the regulations implementing Title VI of the Civil Rights Act of 1964 (Title VI), Section 504 of the Rehabilitation Act of 1973 (Section 504), or Title II of the Americans with Disabilities Act of 1990 (ADA), may contact the Superintendent or Human Resources.
+Garfield School District RE-2 does not discriminate on the basis of race, color, national origin, sex, disability, or age in its programs and activities and provides equal access to the Boy Scouts and other designated your groups.
+The following person has been designated to handle inquiries regarding the non-discrimination policies:
+Superintendent or Director of Human Resources
+839 Whiteriver Ave
+Rifle, CO 81650
+970-665-7600
+For further information on notice of non-discrimination, visit http:wdcrobcolp01.ed.gov/CFAPPS/OCR/contactus.cfm for the address and phone number of the office that serves your area, or call 1-800-421-3481. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>$59,033 /yr (est.)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Delta County School District Elementary School Teacher K-5 Delta, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">insuranceSchedule:8 hour shiftWork Location: Multiple Locations </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">yearBenefits:Dental insuranceFlexible spending accountHealth insuranceLife insurancePaid time offRetirement planVision </x:t>
+  </x:si>
+  <x:si>
+    <x:t>$36,060 /yr (est.)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garfield RE-2 School District 1st Grade Teacher Rifle, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">insuranceSchedule:10 hour shiftDay shiftEducation:Bachelor's (Preferred)License/Certification:Teaching License (Preferred)Work Location: One location </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">experience, and continuing education credits. For out of District experience, the District can honor up to 10 years of out of District experience towards salary credit. Credits for salary advancement can be obtained through professional development, or completing graduate level courses.Garfield Re-2 School District offers </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Benefits Considerations: The salary range for this position is $36,896 - $81,170. Salary is determined by level of education, benefits including medical, dental, and vision coverage, prescription drug coverage, medical and dependent care flexible spending accounts, metlife products, employee assistance programs, surgery plus opportunities, paid time off, sick leave, vacation leave, holiday pay, PERA retirement plan, identity theft protection, local discounts, Verizon Wireless discount, and more.Job Types: Full-time, ContractPay: $36,896.00 - $81,170.00 per yearBenefits:401(k)Dental insuranceEmployee assistance programFlexible spending accountHealth insuranceHealth savings accountLife insurancePaid time offRetirement planVision </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garfield RE-2 School District Special Education Teacher Rifle, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garfield RE-2 School District English Language Learners ELL/ELD Teacher Rifle, CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4th Grade Classroom Teacher BOOKCLIFF CHRISTIAN SCHOOL</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Teaching CertificationTeachingBachelor's degree </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Paid time offHealth insurance Full-timeBenefits:Health insurancePaid time </x:t>
   </x:si>
   <x:si>
     <x:t>IH Services General Cleaner Gene Autry, OK</x:t>
@@ -592,6 +488,9 @@
     <x:t xml:space="preserve">experienceHigh school diploma/GED requiredAbility to successfully pass a back-ground check and pre-employment drug screen. </x:t>
   </x:si>
   <x:si>
+    <x:t>Environmental Svc Tech I Mercy</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">Communication skillsCleaning </x:t>
   </x:si>
   <x:si>
@@ -612,6 +511,9 @@
 At Mercy, our supportive community will be behind you every step of your day, especially the tough ones. You will have opportunities to pioneer new models of care and transform the health care </x:t>
   </x:si>
   <x:si>
+    <x:t>Environ Svc Floor Tech Mercy</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">Communication skillsFloor careOrganizational skillsHigh school diploma or GED procedures.
 Qualifications:
 Education:
@@ -642,6 +544,12 @@
     <x:t xml:space="preserve">Paid time offDental insuranceHealth insuranceEmployee assistance programVision insurance </x:t>
   </x:si>
   <x:si>
+    <x:t>General Cleaner IH Services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nurse Technician-NT - Ardmore 2nd Floor - PRN/Days Mercy</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">Certified Patient Care TechnicianLPNCNAEMT experienceHigh school diploma or GED patient.
 Qualifications:
 Education: High school diploma, G.E.D. and enrolled in a board-certified nursing program. Prior to employment, the nurse tech shall provide student transcripts indicating they have completed Fundamentals of Nursing from an accredited school of nursing and provide competency skills list from their learning institution. The nurse tech must remain in good standing with their school of nursing while in this role. This program is for nursing students only, if a student leaves a program for any reason, they can no longer be a nurse tech.
@@ -670,6 +578,9 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Dental insuranceHealth insuranceEmployee assistance program401(k) matchingPaid time off Part-timeBenefits:401(k)401(k) matchingDental insuranceEmployee assistance programHealth insuranceLife insurancePaid time offVision </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Part-time</x:t>
   </x:si>
   <x:si>
     <x:t>Housekeeper, Maid economy inn express</x:t>
@@ -801,7 +712,10 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="6">
+  <x:cellStyleXfs count="7">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -1171,823 +1085,761 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s"/>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="E2" s="1" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="F2" s="1" t="s"/>
+      <x:c r="G2" s="1" t="s"/>
+      <x:c r="H2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E2" s="1" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="F2" s="1" t="s"/>
-      <x:c r="G2" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="K2" s="0" t="s">
-        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="K3" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="J7" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="K7" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11">
       <x:c r="A8" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="K8" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:11">
       <x:c r="A9" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="J9" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="K9" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:11">
       <x:c r="A10" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="K10" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:11">
       <x:c r="A11" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:11">
       <x:c r="A12" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="H12" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:11">
       <x:c r="A13" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H13" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:11">
       <x:c r="A14" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="J14" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:11">
       <x:c r="A15" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="K15" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:11">
       <x:c r="A16" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="H16" s="0" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="K16" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:11">
       <x:c r="A17" s="0" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="H17" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>41</x:v>
       </x:c>
       <x:c r="J17" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:11">
       <x:c r="A18" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>46</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="J18" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:11">
       <x:c r="A19" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J19" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:11">
       <x:c r="A20" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="J20" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:11">
       <x:c r="A21" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="J21" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:11">
       <x:c r="A22" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="J22" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:11">
       <x:c r="A23" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="J23" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:11">
       <x:c r="A24" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="J24" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="K24" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:11">
       <x:c r="A25" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="J25" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:11">
       <x:c r="A26" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="J26" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:11">
       <x:c r="A27" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="J27" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="K27" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:11">
       <x:c r="A28" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="J28" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:11">
       <x:c r="A29" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:11">
       <x:c r="A30" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="K30" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:11">
       <x:c r="A31" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="K31" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:11">
       <x:c r="A32" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="K32" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:11">
       <x:c r="A33" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:11">
       <x:c r="A34" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="E34" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="K34" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:11">
       <x:c r="A35" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D35" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:11">
       <x:c r="A36" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="E36" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:11">
       <x:c r="A37" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="E37" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:11">
       <x:c r="A38" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E38" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="G38" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="H38" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:11">
       <x:c r="A39" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E39" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="G39" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="H39" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:11">
       <x:c r="A40" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:11">
       <x:c r="A41" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G41" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:11">
       <x:c r="A42" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="E42" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="K42" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:11">
       <x:c r="A43" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E43" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="H43" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:11">
       <x:c r="A44" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D44" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E44" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="H44" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:11">
       <x:c r="A45" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="E45" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F45" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G45" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="H45" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:11">
       <x:c r="A46" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="E46" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G46" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="H46" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:11">
       <x:c r="A47" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D47" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E47" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="G47" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="H47" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:11">
       <x:c r="A48" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="E48" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="H48" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:11">
       <x:c r="A49" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E49" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>